<commit_message>
fixed a wrong data
</commit_message>
<xml_diff>
--- a/Experiment1/phy1011/data.xlsx
+++ b/Experiment1/phy1011/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\programming\python\PhysicsExperiment\Experiment1\phy1011\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57CE4676-4FCF-43BB-8B3C-A6B89F107434}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6411FA4-0931-46B4-922D-F692D3C4A9F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-456" yWindow="708" windowWidth="17280" windowHeight="10320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1524" yWindow="1188" windowWidth="17280" windowHeight="10320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -283,14 +283,26 @@
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -298,20 +310,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -596,7 +596,7 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -607,7 +607,7 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="9" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -619,36 +619,36 @@
       <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="8">
+      <c r="A4" s="10"/>
+      <c r="B4" s="3">
         <v>39.61</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="3">
         <v>39.65</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="3">
         <v>39.630000000000003</v>
       </c>
       <c r="F4" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="8">
-        <v>98.5</v>
+      <c r="G4" s="3">
+        <v>8.5</v>
       </c>
       <c r="H4" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="8">
+      <c r="I4" s="3">
         <v>0.02</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="11" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -665,20 +665,20 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="8">
+      <c r="A6" s="12"/>
+      <c r="B6" s="3">
         <v>111.12</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="3">
         <v>111.13</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="3">
         <v>111.12</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="3">
         <v>9.8011999999999997</v>
       </c>
     </row>
@@ -689,20 +689,20 @@
       <c r="D7" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="3">
         <v>5.8999999999999997E-2</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -734,25 +734,25 @@
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="3">
         <v>0.85499999999999998</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="3">
         <v>0.85399999999999998</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="3">
         <v>0.85399999999999998</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="3">
         <v>0.85599999999999998</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="3">
         <v>0.85799999999999998</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="3">
         <v>0.86899999999999999</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10" s="3">
         <v>0.85499999999999998</v>
       </c>
       <c r="I10" t="s">
@@ -763,25 +763,25 @@
       <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="3">
         <v>0.79600000000000004</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="3">
         <v>0.79500000000000004</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="3">
         <v>0.79500000000000004</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="3">
         <v>0.79700000000000004</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="3">
         <v>0.79900000000000004</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="3">
         <v>0.81</v>
       </c>
-      <c r="H11" s="8">
+      <c r="H11" s="3">
         <v>0.79600000000000004</v>
       </c>
       <c r="I11" t="s">
@@ -789,17 +789,17 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -834,28 +834,28 @@
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="4">
         <v>10</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="4">
         <v>12</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="4">
         <v>14</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="4">
         <v>16</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F15" s="4">
         <v>18</v>
       </c>
-      <c r="G15" s="9">
+      <c r="G15" s="4">
         <v>20</v>
       </c>
-      <c r="H15" s="9">
+      <c r="H15" s="4">
         <v>22</v>
       </c>
-      <c r="I15" s="9">
+      <c r="I15" s="4">
         <v>24</v>
       </c>
     </row>
@@ -863,28 +863,28 @@
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16" s="3">
         <v>6.72</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="3">
         <v>7.21</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D16" s="3">
         <v>7.65</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16" s="3">
         <v>8.11</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F16" s="3">
         <v>8.5500000000000007</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="3">
         <v>8.99</v>
       </c>
-      <c r="H16" s="8">
+      <c r="H16" s="3">
         <v>9.4700000000000006</v>
       </c>
-      <c r="I16" s="8">
+      <c r="I16" s="3">
         <v>9.91</v>
       </c>
     </row>
@@ -892,28 +892,28 @@
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B17" s="3">
         <v>6.74</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17" s="3">
         <v>7.22</v>
       </c>
-      <c r="D17" s="8">
+      <c r="D17" s="3">
         <v>7.64</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17" s="3">
         <v>8.1199999999999992</v>
       </c>
-      <c r="F17" s="8">
+      <c r="F17" s="3">
         <v>8.57</v>
       </c>
-      <c r="G17" s="8">
+      <c r="G17" s="3">
         <v>9.02</v>
       </c>
-      <c r="H17" s="8">
+      <c r="H17" s="3">
         <v>9.48</v>
       </c>
-      <c r="I17" s="8">
+      <c r="I17" s="3">
         <v>9.9</v>
       </c>
     </row>
@@ -921,33 +921,33 @@
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" s="3">
         <v>6.73</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C18" s="3">
         <v>7.2149999999999999</v>
       </c>
-      <c r="D18" s="8">
+      <c r="D18" s="3">
         <v>7.6449999999999996</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E18" s="3">
         <v>8.1150000000000002</v>
       </c>
-      <c r="F18" s="8">
+      <c r="F18" s="3">
         <v>8.56</v>
       </c>
-      <c r="G18" s="8">
+      <c r="G18" s="3">
         <v>9.0050000000000008</v>
       </c>
-      <c r="H18" s="8">
+      <c r="H18" s="3">
         <v>9.4749999999999996</v>
       </c>
-      <c r="I18" s="8">
+      <c r="I18" s="3">
         <v>9.9049999999999994</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="5" t="s">
         <v>28</v>
       </c>
       <c r="D19" t="s">
@@ -955,28 +955,28 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B20" s="12">
+      <c r="B20" s="6">
         <v>2</v>
       </c>
       <c r="D20" t="s">
         <v>25</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E20" s="3">
         <v>0.3</v>
       </c>
       <c r="F20" t="s">
         <v>26</v>
       </c>
-      <c r="G20" s="8">
+      <c r="G20" s="3">
         <v>0.5</v>
       </c>
       <c r="H20" t="s">
         <v>27</v>
       </c>
-      <c r="I20" s="8">
+      <c r="I20" s="3">
         <v>0.02</v>
       </c>
     </row>

</xml_diff>